<commit_message>
Add new testcases and pages
</commit_message>
<xml_diff>
--- a/TestData/AssetHealthPermission.xlsx
+++ b/TestData/AssetHealthPermission.xlsx
@@ -1,33 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SVN\IronIntel\Doc\AutoTest\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FBBA5E-F4E9-4E32-8C4E-DEEA1BE94A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA2E19B6-4571-46EB-8F76-F6B81A90BE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21975" yWindow="1155" windowWidth="18645" windowHeight="12270" xr2:uid="{FF57EAB9-76D8-476B-A96B-8F98C477B7E3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FF57EAB9-76D8-476B-A96B-8F98C477B7E3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -51,103 +42,103 @@
     <t>Alert+WO</t>
   </si>
   <si>
+    <t>Work Order</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>Fuel Records</t>
+  </si>
+  <si>
+    <t>Customer Record</t>
+  </si>
+  <si>
+    <t>Alert+PM</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>WO+Fuel+Customer</t>
+  </si>
+  <si>
+    <t>Work Order,Fuel Records,Customer Record</t>
+  </si>
+  <si>
+    <t>Alert+PM+Fuel+Customer</t>
+  </si>
+  <si>
+    <t>PM+Customer</t>
+  </si>
+  <si>
+    <t>Work Order+Surveys</t>
+  </si>
+  <si>
+    <t>Customer Record + Surveys</t>
+  </si>
+  <si>
+    <t>Customer Record,Customer Satisfaction Surveys,Survey Management/Result,Templates,Report</t>
+  </si>
+  <si>
+    <t>{"UserInfo":{"ID":"atpermission@iicon004.com","DisplayName":"Auto+Test+Permissions","TextAddress":"","Mobile":"","BusinessPhone":"","Active":true,"UserType":"1","IsUser":true,"AllowLoginIntoPC":true,"AllowLoginIntoInspectMobile":false,"AllowLoginIntoFleetMobile":false,"AllowMobileBarcodeScanning":false,"ContactType":"100","ManagerIID":"","Notes":"","AssignedWorkOrders":false,"EmailOptOut":false,"InspectEmailList":false,"TeamIntelligenceUser":false,"FOB":"","HourlyRate":-1,"LandingPage":"MapView.aspx","PreferredLanguage":"","IsAdvisor":false,"LoginVerifyType":"0","LocationIds":[],"DepartmentIds":[],"IID":"5AB99F30-4CC9-4C74-98C0-57A426A72114"},"Subscribe":{"$type":"FI.FIC.Contracts.DataObjects.BaseObject.SubscribeMessageByEmail,+FICIntfAdv","NeedSendMessages":[],"UserEmail":"","UserTextMessage":""},"Features":[{"Key":100,"Value":["99999"]},{"Key":110,"Value":["0"]},{"Key":120,"Value":["0"]},{"Key":130,"Value":["0"]},{"Key":140,"Value":["0"]},{"Key":200,"Value":["99999"]},{"Key":210,"Value":["0"]},{"Key":220,"Value":["0"]},{"Key":230,"Value":["0"]},{"Key":235,"Value":["0"]},{"Key":237,"Value":["0"]},{"Key":245,"Value":["0"]},{"Key":239,"Value":["0"]},{"Key":248,"Value":["0"]},{"Key":300,"Value":["0"]},{"Key":600,"Value":["99999"]},{"Key":601,"Value":["0"]},{"Key":602,"Value":["0"]},{"Key":800,"Value":["99999"]},{"Key":900,"Value":["99999"]},{"Key":1000,"Value":["0"]},{"Key":1100,"Value":["0"]},{"Key":1101,"Value":["0"]}],"Schedule":{"$type":"FI.FIC.EmailSchedule,+FICBLC","ScheduleItems":{"$type":"FI.FIC.EmailScheduleItem[],+FICBLC","$values":[]}}}</t>
+  </si>
+  <si>
+    <t>{"UserInfo":{"ID":"atpermission@iicon004.com","DisplayName":"Auto+Test+Permissions","TextAddress":"","Mobile":"","BusinessPhone":"","Active":true,"UserType":"1","IsUser":true,"AllowLoginIntoPC":true,"AllowLoginIntoInspectMobile":false,"AllowLoginIntoFleetMobile":false,"AllowMobileBarcodeScanning":false,"ContactType":"100","ManagerIID":"","Notes":"","AssignedWorkOrders":false,"EmailOptOut":false,"InspectEmailList":false,"TeamIntelligenceUser":false,"FOB":"","HourlyRate":-1,"LandingPage":"MapView.aspx","PreferredLanguage":"","IsAdvisor":false,"LoginVerifyType":"0","LocationIds":[],"DepartmentIds":[],"IID":"5AB99F30-4CC9-4C74-98C0-57A426A72114"},"Subscribe":{"$type":"FI.FIC.Contracts.DataObjects.BaseObject.SubscribeMessageByEmail,+FICIntfAdv","NeedSendMessages":[],"UserEmail":"","UserTextMessage":""},"Features":[{"Key":100,"Value":["99999"]},{"Key":110,"Value":["0"]},{"Key":120,"Value":["0"]},{"Key":130,"Value":["0"]},{"Key":140,"Value":["0"]},{"Key":200,"Value":["0"]},{"Key":210,"Value":["99999"]},{"Key":220,"Value":["0"]},{"Key":230,"Value":["0"]},{"Key":235,"Value":["0"]},{"Key":237,"Value":["0"]},{"Key":245,"Value":["0"]},{"Key":239,"Value":["0"]},{"Key":248,"Value":["0"]},{"Key":300,"Value":["0"]},{"Key":600,"Value":["99999"]},{"Key":601,"Value":["0"]},{"Key":602,"Value":["0"]},{"Key":800,"Value":["99999"]},{"Key":900,"Value":["99999"]},{"Key":1000,"Value":["0"]},{"Key":1100,"Value":["0"]},{"Key":1101,"Value":["0"]}],"Schedule":{"$type":"FI.FIC.EmailSchedule,+FICBLC","ScheduleItems":{"$type":"FI.FIC.EmailScheduleItem[],+FICBLC","$values":[]}}}</t>
+  </si>
+  <si>
+    <t>{"UserInfo":{"ID":"atpermission@iicon004.com","DisplayName":"Auto+Test+Permissions","TextAddress":"","Mobile":"","BusinessPhone":"","Active":true,"UserType":"1","IsUser":true,"AllowLoginIntoPC":true,"AllowLoginIntoInspectMobile":false,"AllowLoginIntoFleetMobile":false,"AllowMobileBarcodeScanning":false,"ContactType":"100","ManagerIID":"","Notes":"","AssignedWorkOrders":false,"EmailOptOut":false,"InspectEmailList":false,"TeamIntelligenceUser":false,"FOB":"","HourlyRate":-1,"LandingPage":"MapView.aspx","PreferredLanguage":"","IsAdvisor":false,"LoginVerifyType":"0","LocationIds":[],"DepartmentIds":[],"IID":"5AB99F30-4CC9-4C74-98C0-57A426A72114"},"Subscribe":{"$type":"FI.FIC.Contracts.DataObjects.BaseObject.SubscribeMessageByEmail,+FICIntfAdv","NeedSendMessages":[],"UserEmail":"","UserTextMessage":""},"Features":[{"Key":100,"Value":["99999"]},{"Key":110,"Value":["0"]},{"Key":120,"Value":["0"]},{"Key":130,"Value":["0"]},{"Key":140,"Value":["0"]},{"Key":200,"Value":["0"]},{"Key":210,"Value":["0"]},{"Key":220,"Value":["99999"]},{"Key":230,"Value":["0"]},{"Key":235,"Value":["0"]},{"Key":237,"Value":["0"]},{"Key":245,"Value":["0"]},{"Key":239,"Value":["0"]},{"Key":248,"Value":["0"]},{"Key":300,"Value":["0"]},{"Key":600,"Value":["99999"]},{"Key":601,"Value":["0"]},{"Key":602,"Value":["0"]},{"Key":800,"Value":["99999"]},{"Key":900,"Value":["99999"]},{"Key":1000,"Value":["0"]},{"Key":1100,"Value":["0"]},{"Key":1101,"Value":["0"]}],"Schedule":{"$type":"FI.FIC.EmailSchedule,+FICBLC","ScheduleItems":{"$type":"FI.FIC.EmailScheduleItem[],+FICBLC","$values":[]}}}</t>
+  </si>
+  <si>
+    <t>{"UserInfo":{"ID":"atpermission@iicon004.com","DisplayName":"Auto+Test+Permissions","TextAddress":"","Mobile":"","BusinessPhone":"","Active":true,"UserType":"1","IsUser":true,"AllowLoginIntoPC":true,"AllowLoginIntoInspectMobile":false,"AllowLoginIntoFleetMobile":false,"AllowMobileBarcodeScanning":false,"ContactType":"100","ManagerIID":"","Notes":"","AssignedWorkOrders":false,"EmailOptOut":false,"InspectEmailList":false,"TeamIntelligenceUser":false,"FOB":"","HourlyRate":-1,"LandingPage":"MapView.aspx","PreferredLanguage":"","IsAdvisor":false,"LoginVerifyType":"0","LoginVerifyType":"0","LocationIds":[],"DepartmentIds":[],"IID":"5AB99F30-4CC9-4C74-98C0-57A426A72114"},"Subscribe":{"$type":"FI.FIC.Contracts.DataObjects.BaseObject.SubscribeMessageByEmail,+FICIntfAdv","NeedSendMessages":[],"UserEmail":"","UserTextMessage":""},"Features":[{"Key":100,"Value":["99999"]},{"Key":110,"Value":["0"]},{"Key":120,"Value":["0"]},{"Key":130,"Value":["0"]},{"Key":140,"Value":["0"]},{"Key":200,"Value":["0"]},{"Key":210,"Value":["0"]},{"Key":220,"Value":["0"]},{"Key":230,"Value":["99999"]},{"Key":235,"Value":["0"]},{"Key":237,"Value":["0"]},{"Key":245,"Value":["0"]},{"Key":239,"Value":["0"]},{"Key":248,"Value":["0"]},{"Key":300,"Value":["0"]},{"Key":600,"Value":["99999"]},{"Key":601,"Value":["0"]},{"Key":602,"Value":["0"]},{"Key":800,"Value":["99999"]},{"Key":900,"Value":["99999"]},{"Key":1000,"Value":["0"]},{"Key":1100,"Value":["0"]},{"Key":1101,"Value":["0"]}],"Schedule":{"$type":"FI.FIC.EmailSchedule,+FICBLC","ScheduleItems":{"$type":"FI.FIC.EmailScheduleItem[],+FICBLC","$values":[]}}}</t>
+  </si>
+  <si>
+    <t>{"UserInfo":{"ID":"atpermission@iicon004.com","DisplayName":"Auto+Test+Permissions","TextAddress":"","Mobile":"","BusinessPhone":"","Active":true,"UserType":"1","IsUser":true,"AllowLoginIntoPC":true,"AllowLoginIntoInspectMobile":false,"AllowLoginIntoFleetMobile":false,"AllowMobileBarcodeScanning":false,"ContactType":"100","ManagerIID":"","Notes":"","AssignedWorkOrders":false,"EmailOptOut":false,"InspectEmailList":false,"TeamIntelligenceUser":false,"FOB":"","HourlyRate":-1,"LandingPage":"MapView.aspx","PreferredLanguage":"","LoginVerifyType":"0","LocationIds":[],"DepartmentIds":[],"IID":"5AB99F30-4CC9-4C74-98C0-57A426A72114"},"Subscribe":{"$type":"FI.FIC.Contracts.DataObjects.BaseObject.SubscribeMessageByEmail, FICIntfAdv","NeedSendMessages":[],"UserEmail":"","UserTextMessage":""},"Features":[{"Key":100,"Value":["99999"]},{"Key":110,"Value":["0"]},{"Key":120,"Value":["0"]},{"Key":130,"Value":["0"]},{"Key":140,"Value":["0"]},{"Key":200,"Value":["0"]},{"Key":210,"Value":["0"]},{"Key":220,"Value":["0"]},{"Key":230,"Value":["0"]},{"Key":235,"Value":["99999"]},{"Key":237,"Value":["0"]},{"Key":245,"Value":["0"]},{"Key":239,"Value":["0"]},{"Key":248,"Value":["0"]},{"Key":300,"Value":["0"]},{"Key":600,"Value":["99999"]},{"Key":601,"Value":["0"]},{"Key":602,"Value":["0"]},{"Key":800,"Value":["0"]},{"Key":900,"Value":["0"]},{"Key":1000,"Value":["99999"]},{"Key":1100,"Value":["99999"]},{"Key":1101,"Value":["0"]}],"Schedule":{"$type":"FI.FIC.EmailSchedule, FICBLC","ScheduleItems":{"$type":"FI.FIC.EmailScheduleItem[], FICBLC","$values":[]}}}</t>
+  </si>
+  <si>
+    <t>{"UserInfo":{"ID":"atpermission@iicon004.com","DisplayName":"Auto+Test+Permissions","TextAddress":"","Mobile":"","BusinessPhone":"","Active":true,"UserType":"1","IsUser":true,"AllowLoginIntoPC":true,"AllowLoginIntoInspectMobile":false,"AllowLoginIntoFleetMobile":false,"AllowMobileBarcodeScanning":false,"ContactType":"100","ManagerIID":"","Notes":"","AssignedWorkOrders":false,"EmailOptOut":false,"InspectEmailList":false,"TeamIntelligenceUser":false,"FOB":"","HourlyRate":-1,"LandingPage":"MapView.aspx","PreferredLanguage":"","IsAdvisor":false,"LoginVerifyType":"0","LocationIds":[],"DepartmentIds":[],"IID":"5AB99F30-4CC9-4C74-98C0-57A426A72114"},"Subscribe":{"$type":"FI.FIC.Contracts.DataObjects.BaseObject.SubscribeMessageByEmail,+FICIntfAdv","NeedSendMessages":[],"UserEmail":"","UserTextMessage":""},"Features":[{"Key":100,"Value":["99999"]},{"Key":110,"Value":["0"]},{"Key":120,"Value":["0"]},{"Key":130,"Value":["0"]},{"Key":140,"Value":["0"]},{"Key":200,"Value":["99999"]},{"Key":210,"Value":["99999"]},{"Key":220,"Value":["0"]},{"Key":230,"Value":["0"]},{"Key":235,"Value":["0"]},{"Key":237,"Value":["0"]},{"Key":245,"Value":["0"]},{"Key":239,"Value":["0"]},{"Key":248,"Value":["0"]},{"Key":300,"Value":["0"]},{"Key":600,"Value":["99999"]},{"Key":601,"Value":["0"]},{"Key":602,"Value":["0"]},{"Key":800,"Value":["99999"]},{"Key":900,"Value":["99999"]},{"Key":1000,"Value":["0"]},{"Key":1100,"Value":["0"]},{"Key":1101,"Value":["0"]}],"Schedule":{"$type":"FI.FIC.EmailSchedule,+FICBLC","ScheduleItems":{"$type":"FI.FIC.EmailScheduleItem[],+FICBLC","$values":[]}}}</t>
+  </si>
+  <si>
+    <t>{"UserInfo":{"ID":"atpermission@iicon004.com","DisplayName":"Auto+Test+Permissions","TextAddress":"","Mobile":"","BusinessPhone":"","Active":true,"UserType":"1","IsUser":true,"AllowLoginIntoPC":true,"AllowLoginIntoInspectMobile":false,"AllowLoginIntoFleetMobile":false,"AllowMobileBarcodeScanning":false,"ContactType":"100","ManagerIID":"","Notes":"","AssignedWorkOrders":false,"EmailOptOut":false,"InspectEmailList":false,"TeamIntelligenceUser":false,"FOB":"","HourlyRate":-1,"LandingPage":"MapView.aspx","PreferredLanguage":"","IsAdvisor":false,"LoginVerifyType":"0","LocationIds":[],"DepartmentIds":[],"IID":"5AB99F30-4CC9-4C74-98C0-57A426A72114"},"Subscribe":{"$type":"FI.FIC.Contracts.DataObjects.BaseObject.SubscribeMessageByEmail,+FICIntfAdv","NeedSendMessages":[],"UserEmail":"","UserTextMessage":""},"Features":[{"Key":100,"Value":["99999"]},{"Key":110,"Value":["0"]},{"Key":120,"Value":["0"]},{"Key":130,"Value":["0"]},{"Key":140,"Value":["0"]},{"Key":200,"Value":["99999"]},{"Key":210,"Value":["0"]},{"Key":220,"Value":["99999"]},{"Key":230,"Value":["0"]},{"Key":235,"Value":["0"]},{"Key":237,"Value":["0"]},{"Key":245,"Value":["0"]},{"Key":239,"Value":["0"]},{"Key":248,"Value":["0"]},{"Key":300,"Value":["0"]},{"Key":600,"Value":["99999"]},{"Key":601,"Value":["0"]},{"Key":602,"Value":["0"]},{"Key":800,"Value":["99999"]},{"Key":900,"Value":["99999"]},{"Key":1000,"Value":["0"]},{"Key":1100,"Value":["0"]},{"Key":1101,"Value":["0"]}],"Schedule":{"$type":"FI.FIC.EmailSchedule,+FICBLC","ScheduleItems":{"$type":"FI.FIC.EmailScheduleItem[],+FICBLC","$values":[]}}}</t>
+  </si>
+  <si>
+    <t>{"UserInfo":{"ID":"atpermission@iicon004.com","DisplayName":"Auto+Test+Permissions","TextAddress":"","Mobile":"","BusinessPhone":"","Active":true,"UserType":"1","IsUser":true,"AllowLoginIntoPC":true,"AllowLoginIntoInspectMobile":false,"AllowLoginIntoFleetMobile":false,"AllowMobileBarcodeScanning":false,"ContactType":"100","ManagerIID":"","Notes":"","AssignedWorkOrders":false,"EmailOptOut":false,"InspectEmailList":false,"TeamIntelligenceUser":false,"FOB":"","HourlyRate":-1,"LandingPage":"MapView.aspx","PreferredLanguage":"","LoginVerifyType":"0","LocationIds":[],"DepartmentIds":[],"IID":"5AB99F30-4CC9-4C74-98C0-57A426A72114"},"Subscribe":{"$type":"FI.FIC.Contracts.DataObjects.BaseObject.SubscribeMessageByEmail, FICIntfAdv","NeedSendMessages":[],"UserEmail":"","UserTextMessage":""},"Features":[{"Key":100,"Value":["99999"]},{"Key":110,"Value":["0"]},{"Key":120,"Value":["0"]},{"Key":130,"Value":["0"]},{"Key":140,"Value":["0"]},{"Key":200,"Value":["0"]},{"Key":210,"Value":["0"]},{"Key":220,"Value":["99999"]},{"Key":230,"Value":["0"]},{"Key":235,"Value":["99999"]},{"Key":237,"Value":["0"]},{"Key":245,"Value":["0"]},{"Key":239,"Value":["0"]},{"Key":248,"Value":["0"]},{"Key":300,"Value":["0"]},{"Key":600,"Value":["99999"]},{"Key":601,"Value":["0"]},{"Key":602,"Value":["0"]},{"Key":800,"Value":["0"]},{"Key":900,"Value":["0"]},{"Key":1000,"Value":["99999"]},{"Key":1100,"Value":["99999"]},{"Key":1101,"Value":["0"]}],"Schedule":{"$type":"FI.FIC.EmailSchedule, FICBLC","ScheduleItems":{"$type":"FI.FIC.EmailScheduleItem[], FICBLC","$values":[]}}}</t>
+  </si>
+  <si>
+    <t>{"UserInfo":{"ID":"atpermission@iicon004.com","DisplayName":"Auto+Test+Permissions","TextAddress":"","Mobile":"","BusinessPhone":"","Active":true,"UserType":"1","IsUser":true,"AllowLoginIntoPC":true,"AllowLoginIntoInspectMobile":false,"AllowLoginIntoFleetMobile":false,"AllowMobileBarcodeScanning":false,"ContactType":"100","ManagerIID":"","Notes":"","AssignedWorkOrders":false,"EmailOptOut":false,"InspectEmailList":false,"TeamIntelligenceUser":false,"FOB":"","HourlyRate":-1,"LandingPage":"MapView.aspx","PreferredLanguage":"","LoginVerifyType":"0","LocationIds":[],"DepartmentIds":[],"IID":"5AB99F30-4CC9-4C74-98C0-57A426A72114"},"Subscribe":{"$type":"FI.FIC.Contracts.DataObjects.BaseObject.SubscribeMessageByEmail, FICIntfAdv","NeedSendMessages":[],"UserEmail":"","UserTextMessage":""},"Features":[{"Key":100,"Value":["99999"]},{"Key":110,"Value":["0"]},{"Key":120,"Value":["0"]},{"Key":130,"Value":["0"]},{"Key":140,"Value":["0"]},{"Key":200,"Value":["0"]},{"Key":210,"Value":["99999"]},{"Key":220,"Value":["0"]},{"Key":230,"Value":["0"]},{"Key":235,"Value":["0"]},{"Key":237,"Value":["0"]},{"Key":245,"Value":["0"]},{"Key":239,"Value":["0"]},{"Key":248,"Value":["99999"]},{"Key":300,"Value":["0"]},{"Key":600,"Value":["99999"]},{"Key":601,"Value":["0"]},{"Key":602,"Value":["0"]},{"Key":800,"Value":["0"]},{"Key":900,"Value":["0"]},{"Key":1000,"Value":["99999"]},{"Key":1100,"Value":["99999"]},{"Key":1101,"Value":["0"]}],"Schedule":{"$type":"FI.FIC.EmailSchedule, FICBLC","ScheduleItems":{"$type":"FI.FIC.EmailScheduleItem[], FICBLC","$values":[]}}}</t>
+  </si>
+  <si>
+    <t>{"UserInfo":{"ID":"atpermission@iicon004.com","DisplayName":"Auto+Test+Permissions","TextAddress":"","Mobile":"","BusinessPhone":"","Active":true,"UserType":"1","IsUser":true,"AllowLoginIntoPC":true,"AllowLoginIntoInspectMobile":false,"AllowLoginIntoFleetMobile":false,"AllowMobileBarcodeScanning":false,"ContactType":"100","ManagerIID":"","Notes":"","AssignedWorkOrders":false,"EmailOptOut":false,"InspectEmailList":false,"TeamIntelligenceUser":false,"FOB":"","HourlyRate":-1,"LandingPage":"MapView.aspx","PreferredLanguage":"","LoginVerifyType":"0","LocationIds":[],"DepartmentIds":[],"IID":"5AB99F30-4CC9-4C74-98C0-57A426A72114"},"Subscribe":{"$type":"FI.FIC.Contracts.DataObjects.BaseObject.SubscribeMessageByEmail, FICIntfAdv","NeedSendMessages":[],"UserEmail":"","UserTextMessage":""},"Features":[{"Key":100,"Value":["99999"]},{"Key":110,"Value":["0"]},{"Key":120,"Value":["0"]},{"Key":130,"Value":["0"]},{"Key":140,"Value":["0"]},{"Key":200,"Value":["0"]},{"Key":210,"Value":["0"]},{"Key":220,"Value":["0"]},{"Key":230,"Value":["0"]},{"Key":235,"Value":["99999"]},{"Key":237,"Value":["0"]},{"Key":245,"Value":["0"]},{"Key":239,"Value":["0"]},{"Key":248,"Value":["99999"]},{"Key":300,"Value":["0"]},{"Key":600,"Value":["99999"]},{"Key":601,"Value":["0"]},{"Key":602,"Value":["0"]},{"Key":800,"Value":["0"]},{"Key":900,"Value":["0"]},{"Key":1000,"Value":["99999"]},{"Key":1100,"Value":["99999"]},{"Key":1101,"Value":["0"]}],"Schedule":{"$type":"FI.FIC.EmailSchedule, FICBLC","ScheduleItems":{"$type":"FI.FIC.EmailScheduleItem[], FICBLC","$values":[]}}}</t>
+  </si>
+  <si>
+    <t>{"UserInfo":{"ID":"atpermission@iicon004.com","DisplayName":"Auto+Test+Permissions","TextAddress":"","Mobile":"","BusinessPhone":"","Active":true,"UserType":"1","IsUser":true,"AllowLoginIntoPC":true,"AllowLoginIntoInspectMobile":false,"AllowLoginIntoFleetMobile":false,"AllowMobileBarcodeScanning":false,"ContactType":"100","ManagerIID":"","Notes":"","AssignedWorkOrders":false,"EmailOptOut":false,"InspectEmailList":false,"TeamIntelligenceUser":false,"FOB":"","HourlyRate":-1,"LandingPage":"MapView.aspx","PreferredLanguage":"","LoginVerifyType":"0","LocationIds":[],"DepartmentIds":[],"IID":"5AB99F30-4CC9-4C74-98C0-57A426A72114"},"Subscribe":{"$type":"FI.FIC.Contracts.DataObjects.BaseObject.SubscribeMessageByEmail, FICIntfAdv","NeedSendMessages":[],"UserEmail":"","UserTextMessage":""},"Features":[{"Key":100,"Value":["99999"]},{"Key":110,"Value":["0"]},{"Key":120,"Value":["0"]},{"Key":130,"Value":["0"]},{"Key":140,"Value":["0"]},{"Key":200,"Value":["0"]},{"Key":210,"Value":["99999"]},{"Key":220,"Value":["0"]},{"Key":230,"Value":["99999"]},{"Key":235,"Value":["99999"]},{"Key":237,"Value":["0"]},{"Key":245,"Value":["0"]},{"Key":239,"Value":["0"]},{"Key":248,"Value":["0"]},{"Key":300,"Value":["0"]},{"Key":600,"Value":["99999"]},{"Key":601,"Value":["0"]},{"Key":602,"Value":["0"]},{"Key":800,"Value":["0"]},{"Key":900,"Value":["0"]},{"Key":1000,"Value":["99999"]},{"Key":1100,"Value":["99999"]},{"Key":1101,"Value":["0"]}],"Schedule":{"$type":"FI.FIC.EmailSchedule, FICBLC","ScheduleItems":{"$type":"FI.FIC.EmailScheduleItem[], FICBLC","$values":[]}}}</t>
+  </si>
+  <si>
+    <t>{"UserInfo":{"ID":"atpermission@iicon004.com","DisplayName":"Auto+Test+Permissions","TextAddress":"","Mobile":"","BusinessPhone":"","Active":true,"UserType":"1","IsUser":true,"AllowLoginIntoPC":true,"AllowLoginIntoInspectMobile":false,"AllowLoginIntoFleetMobile":false,"AllowMobileBarcodeScanning":false,"ContactType":"100","ManagerIID":"","Notes":"","AssignedWorkOrders":false,"EmailOptOut":false,"InspectEmailList":false,"TeamIntelligenceUser":false,"FOB":"","HourlyRate":-1,"LandingPage":"MapView.aspx","PreferredLanguage":"","LoginVerifyType":"0","LocationIds":[],"DepartmentIds":[],"IID":"5AB99F30-4CC9-4C74-98C0-57A426A72114"},"Subscribe":{"$type":"FI.FIC.Contracts.DataObjects.BaseObject.SubscribeMessageByEmail, FICIntfAdv","NeedSendMessages":[],"UserEmail":"","UserTextMessage":""},"Features":[{"Key":100,"Value":["99999"]},{"Key":110,"Value":["0"]},{"Key":120,"Value":["0"]},{"Key":130,"Value":["0"]},{"Key":140,"Value":["0"]},{"Key":200,"Value":["99999"]},{"Key":210,"Value":["0"]},{"Key":220,"Value":["99999"]},{"Key":230,"Value":["99999"]},{"Key":235,"Value":["99999"]},{"Key":237,"Value":["0"]},{"Key":245,"Value":["0"]},{"Key":239,"Value":["0"]},{"Key":248,"Value":["0"]},{"Key":300,"Value":["0"]},{"Key":600,"Value":["99999"]},{"Key":601,"Value":["0"]},{"Key":602,"Value":["0"]},{"Key":800,"Value":["0"]},{"Key":900,"Value":["0"]},{"Key":1000,"Value":["99999"]},{"Key":1100,"Value":["99999"]},{"Key":1101,"Value":["0"]}],"Schedule":{"$type":"FI.FIC.EmailSchedule, FICBLC","ScheduleItems":{"$type":"FI.FIC.EmailScheduleItem[], FICBLC","$values":[]}}}</t>
+  </si>
+  <si>
+    <t>{"UserInfo":{"ID":"atpermission@iicon004.com","DisplayName":"Auto+Test+Permissions","TextAddress":"","Mobile":"","BusinessPhone":"","Active":true,"UserType":"1","IsUser":true,"AllowLoginIntoPC":true,"AllowLoginIntoInspectMobile":false,"AllowLoginIntoFleetMobile":false,"AllowMobileBarcodeScanning":false,"ContactType":"100","ManagerIID":"","Notes":"","AssignedWorkOrders":false,"EmailOptOut":false,"InspectEmailList":false,"TeamIntelligenceUser":false,"FOB":"","HourlyRate":-1,"LandingPage":"MapView.aspx","PreferredLanguage":"","LoginVerifyType":"0","LocationIds":[],"DepartmentIds":[],"IID":"5AB99F30-4CC9-4C74-98C0-57A426A72114"},"Subscribe":{"$type":"FI.FIC.Contracts.DataObjects.BaseObject.SubscribeMessageByEmail, FICIntfAdv","NeedSendMessages":[],"UserEmail":"","UserTextMessage":""},"Features":[{"Key":100,"Value":["99999"]},{"Key":110,"Value":["0"]},{"Key":120,"Value":["0"]},{"Key":130,"Value":["0"]},{"Key":140,"Value":["0"]},{"Key":200,"Value":["99999"]},{"Key":210,"Value":["99999"]},{"Key":220,"Value":["99999"]},{"Key":230,"Value":["99999"]},{"Key":235,"Value":["99999"]},{"Key":237,"Value":["99999"]},{"Key":245,"Value":["99999"]},{"Key":239,"Value":["99999"]},{"Key":248,"Value":["99999"]},{"Key":300,"Value":["0"]},{"Key":600,"Value":["99999"]},{"Key":601,"Value":["0"]},{"Key":602,"Value":["0"]},{"Key":800,"Value":["0"]},{"Key":900,"Value":["0"]},{"Key":1000,"Value":["99999"]},{"Key":1100,"Value":["99999"]},{"Key":1101,"Value":["0"]}],"Schedule":{"$type":"FI.FIC.EmailSchedule, FICBLC","ScheduleItems":{"$type":"FI.FIC.EmailScheduleItem[], FICBLC","$values":[]}}}</t>
+  </si>
+  <si>
     <t>Alerts Management</t>
   </si>
   <si>
-    <t>Work Order</t>
-  </si>
-  <si>
-    <t>PM</t>
-  </si>
-  <si>
-    <t>Fuel Records</t>
-  </si>
-  <si>
-    <t>Customer Record</t>
-  </si>
-  <si>
-    <t>Alert+PM</t>
-  </si>
-  <si>
-    <t>Alerts Management,Maintenance Schedules,Maintenance Record</t>
-  </si>
-  <si>
-    <t>Maintenance Schedules,Maintenance Record</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>WO+Fuel+Customer</t>
-  </si>
-  <si>
-    <t>Work Order,Fuel Records,Customer Record</t>
-  </si>
-  <si>
-    <t>Alert+PM+Fuel+Customer</t>
-  </si>
-  <si>
-    <t>Alerts Management,Maintenance Schedules,Maintenance Record,Fuel Records,Customer Record</t>
-  </si>
-  <si>
-    <t>PM+Customer</t>
-  </si>
-  <si>
-    <t>Maintenance Schedules,Maintenance Record,Customer Record</t>
-  </si>
-  <si>
     <t>Work Order,Alerts Management</t>
   </si>
   <si>
-    <t>Work Order+Surveys</t>
-  </si>
-  <si>
-    <t>Customer Record + Surveys</t>
-  </si>
-  <si>
-    <t>{"UserInfo":{"ID":"atpermission@iicon004.com","DisplayName":"Auto+Test+Permissions","TextAddress":"","Mobile":"","BusinessPhone":"","Active":true,"UserType":"1","IsUser":true,"AllowLoginIntoPC":true,"AllowLoginIntoInspectMobile":false,"AllowLoginIntoFleetMobile":false,"AllowMobileBarcodeScanning":false,"ContactType":"100","ManagerIID":"","Notes":"","AssignedWorkOrders":false,"EmailOptOut":false,"InspectEmailList":false,"TeamIntelligenceUser":false,"FOB":"","HourlyRate":-1,"LandingPage":"MapView.aspx","PreferredLanguage":"","LocationIds":[],"DepartmentIds":[],"IID":"5AB99F30-4CC9-4C74-98C0-57A426A72114"},"Subscribe":{"$type":"FI.FIC.Contracts.DataObjects.BaseObject.SubscribeMessageByEmail, FICIntfAdv","NeedSendMessages":[],"UserEmail":"","UserTextMessage":""},"Features":[{"Key":100,"Value":["99999"]},{"Key":110,"Value":["0"]},{"Key":120,"Value":["0"]},{"Key":130,"Value":["0"]},{"Key":140,"Value":["0"]},{"Key":200,"Value":["0"]},{"Key":210,"Value":["99999"]},{"Key":220,"Value":["0"]},{"Key":230,"Value":["0"]},{"Key":235,"Value":["0"]},{"Key":237,"Value":["0"]},{"Key":245,"Value":["0"]},{"Key":239,"Value":["0"]},{"Key":248,"Value":["99999"]},{"Key":300,"Value":["0"]},{"Key":600,"Value":["99999"]},{"Key":601,"Value":["0"]},{"Key":602,"Value":["0"]},{"Key":800,"Value":["0"]},{"Key":900,"Value":["0"]},{"Key":1000,"Value":["99999"]},{"Key":1100,"Value":["99999"]},{"Key":1101,"Value":["0"]}],"Schedule":{"$type":"FI.FIC.EmailSchedule, FICBLC","ScheduleItems":{"$type":"FI.FIC.EmailScheduleItem[], FICBLC","$values":[]}}}</t>
-  </si>
-  <si>
-    <t>{"UserInfo":{"ID":"atpermission@iicon004.com","DisplayName":"Auto+Test+Permissions","TextAddress":"","Mobile":"","BusinessPhone":"","Active":true,"UserType":"1","IsUser":true,"AllowLoginIntoPC":true,"AllowLoginIntoInspectMobile":false,"AllowLoginIntoFleetMobile":false,"AllowMobileBarcodeScanning":false,"ContactType":"100","ManagerIID":"","Notes":"","AssignedWorkOrders":false,"EmailOptOut":false,"InspectEmailList":false,"TeamIntelligenceUser":false,"FOB":"","HourlyRate":-1,"LandingPage":"MapView.aspx","PreferredLanguage":"","LocationIds":[],"DepartmentIds":[],"IID":"5AB99F30-4CC9-4C74-98C0-57A426A72114"},"Subscribe":{"$type":"FI.FIC.Contracts.DataObjects.BaseObject.SubscribeMessageByEmail, FICIntfAdv","NeedSendMessages":[],"UserEmail":"","UserTextMessage":""},"Features":[{"Key":100,"Value":["99999"]},{"Key":110,"Value":["0"]},{"Key":120,"Value":["0"]},{"Key":130,"Value":["0"]},{"Key":140,"Value":["0"]},{"Key":200,"Value":["0"]},{"Key":210,"Value":["0"]},{"Key":220,"Value":["0"]},{"Key":230,"Value":["0"]},{"Key":235,"Value":["99999"]},{"Key":237,"Value":["0"]},{"Key":245,"Value":["0"]},{"Key":239,"Value":["0"]},{"Key":248,"Value":["99999"]},{"Key":300,"Value":["0"]},{"Key":600,"Value":["99999"]},{"Key":601,"Value":["0"]},{"Key":602,"Value":["0"]},{"Key":800,"Value":["0"]},{"Key":900,"Value":["0"]},{"Key":1000,"Value":["99999"]},{"Key":1100,"Value":["99999"]},{"Key":1101,"Value":["0"]}],"Schedule":{"$type":"FI.FIC.EmailSchedule, FICBLC","ScheduleItems":{"$type":"FI.FIC.EmailScheduleItem[], FICBLC","$values":[]}}}</t>
-  </si>
-  <si>
-    <t>Customer Record,Customer Satisfaction Surveys,Survey Management/Result,Templates</t>
-  </si>
-  <si>
-    <t>{"UserInfo":{"ID":"atpermission@iicon004.com","DisplayName":"Auto+Test+Permissions","TextAddress":"","Mobile":"","BusinessPhone":"","Active":true,"UserType":"1","IsUser":true,"AllowLoginIntoPC":true,"AllowLoginIntoInspectMobile":false,"AllowLoginIntoFleetMobile":false,"AllowMobileBarcodeScanning":false,"ContactType":"100","ManagerIID":"","Notes":"","AssignedWorkOrders":false,"EmailOptOut":false,"InspectEmailList":false,"TeamIntelligenceUser":false,"FOB":"","HourlyRate":-1,"LandingPage":"MapView.aspx","PreferredLanguage":"","LocationIds":[],"DepartmentIds":[],"IID":"5AB99F30-4CC9-4C74-98C0-57A426A72114"},"Subscribe":{"$type":"FI.FIC.Contracts.DataObjects.BaseObject.SubscribeMessageByEmail, FICIntfAdv","NeedSendMessages":[],"UserEmail":"","UserTextMessage":""},"Features":[{"Key":100,"Value":["99999"]},{"Key":110,"Value":["0"]},{"Key":120,"Value":["0"]},{"Key":130,"Value":["0"]},{"Key":140,"Value":["0"]},{"Key":200,"Value":["0"]},{"Key":210,"Value":["0"]},{"Key":220,"Value":["0"]},{"Key":230,"Value":["0"]},{"Key":235,"Value":["99999"]},{"Key":237,"Value":["0"]},{"Key":245,"Value":["0"]},{"Key":239,"Value":["0"]},{"Key":248,"Value":["0"]},{"Key":300,"Value":["0"]},{"Key":600,"Value":["99999"]},{"Key":601,"Value":["0"]},{"Key":602,"Value":["0"]},{"Key":800,"Value":["0"]},{"Key":900,"Value":["0"]},{"Key":1000,"Value":["99999"]},{"Key":1100,"Value":["99999"]},{"Key":1101,"Value":["0"]}],"Schedule":{"$type":"FI.FIC.EmailSchedule, FICBLC","ScheduleItems":{"$type":"FI.FIC.EmailScheduleItem[], FICBLC","$values":[]}}}</t>
-  </si>
-  <si>
-    <t>{"UserInfo":{"ID":"atpermission@iicon004.com","DisplayName":"Auto+Test+Permissions","TextAddress":"","Mobile":"","BusinessPhone":"","Active":true,"UserType":"1","IsUser":true,"AllowLoginIntoPC":true,"AllowLoginIntoInspectMobile":false,"AllowLoginIntoFleetMobile":false,"AllowMobileBarcodeScanning":false,"ContactType":"100","ManagerIID":"","Notes":"","AssignedWorkOrders":false,"EmailOptOut":false,"InspectEmailList":false,"TeamIntelligenceUser":false,"FOB":"","HourlyRate":-1,"LandingPage":"MapView.aspx","PreferredLanguage":"","LocationIds":[],"DepartmentIds":[],"IID":"5AB99F30-4CC9-4C74-98C0-57A426A72114"},"Subscribe":{"$type":"FI.FIC.Contracts.DataObjects.BaseObject.SubscribeMessageByEmail, FICIntfAdv","NeedSendMessages":[],"UserEmail":"","UserTextMessage":""},"Features":[{"Key":100,"Value":["99999"]},{"Key":110,"Value":["0"]},{"Key":120,"Value":["0"]},{"Key":130,"Value":["0"]},{"Key":140,"Value":["0"]},{"Key":200,"Value":["0"]},{"Key":210,"Value":["0"]},{"Key":220,"Value":["99999"]},{"Key":230,"Value":["0"]},{"Key":235,"Value":["99999"]},{"Key":237,"Value":["0"]},{"Key":245,"Value":["0"]},{"Key":239,"Value":["0"]},{"Key":248,"Value":["0"]},{"Key":300,"Value":["0"]},{"Key":600,"Value":["99999"]},{"Key":601,"Value":["0"]},{"Key":602,"Value":["0"]},{"Key":800,"Value":["0"]},{"Key":900,"Value":["0"]},{"Key":1000,"Value":["99999"]},{"Key":1100,"Value":["99999"]},{"Key":1101,"Value":["0"]}],"Schedule":{"$type":"FI.FIC.EmailSchedule, FICBLC","ScheduleItems":{"$type":"FI.FIC.EmailScheduleItem[], FICBLC","$values":[]}}}</t>
-  </si>
-  <si>
-    <t>{"UserInfo":{"ID":"atpermission@iicon004.com","DisplayName":"Auto+Test+Permissions","TextAddress":"","Mobile":"","BusinessPhone":"","Active":true,"UserType":"1","IsUser":true,"AllowLoginIntoPC":true,"AllowLoginIntoInspectMobile":false,"AllowLoginIntoFleetMobile":false,"AllowMobileBarcodeScanning":false,"ContactType":"100","ManagerIID":"","Notes":"","AssignedWorkOrders":false,"EmailOptOut":false,"InspectEmailList":false,"TeamIntelligenceUser":false,"FOB":"","HourlyRate":-1,"LandingPage":"MapView.aspx","PreferredLanguage":"","LocationIds":[],"DepartmentIds":[],"IID":"5AB99F30-4CC9-4C74-98C0-57A426A72114"},"Subscribe":{"$type":"FI.FIC.Contracts.DataObjects.BaseObject.SubscribeMessageByEmail, FICIntfAdv","NeedSendMessages":[],"UserEmail":"","UserTextMessage":""},"Features":[{"Key":100,"Value":["99999"]},{"Key":110,"Value":["0"]},{"Key":120,"Value":["0"]},{"Key":130,"Value":["0"]},{"Key":140,"Value":["0"]},{"Key":200,"Value":["0"]},{"Key":210,"Value":["99999"]},{"Key":220,"Value":["0"]},{"Key":230,"Value":["99999"]},{"Key":235,"Value":["99999"]},{"Key":237,"Value":["0"]},{"Key":245,"Value":["0"]},{"Key":239,"Value":["0"]},{"Key":248,"Value":["0"]},{"Key":300,"Value":["0"]},{"Key":600,"Value":["99999"]},{"Key":601,"Value":["0"]},{"Key":602,"Value":["0"]},{"Key":800,"Value":["0"]},{"Key":900,"Value":["0"]},{"Key":1000,"Value":["99999"]},{"Key":1100,"Value":["99999"]},{"Key":1101,"Value":["0"]}],"Schedule":{"$type":"FI.FIC.EmailSchedule, FICBLC","ScheduleItems":{"$type":"FI.FIC.EmailScheduleItem[], FICBLC","$values":[]}}}</t>
-  </si>
-  <si>
-    <t>{"UserInfo":{"ID":"atpermission@iicon004.com","DisplayName":"Auto+Test+Permissions","TextAddress":"","Mobile":"","BusinessPhone":"","Active":true,"UserType":"1","IsUser":true,"AllowLoginIntoPC":true,"AllowLoginIntoInspectMobile":false,"AllowLoginIntoFleetMobile":false,"AllowMobileBarcodeScanning":false,"ContactType":"100","ManagerIID":"","Notes":"","AssignedWorkOrders":false,"EmailOptOut":false,"InspectEmailList":false,"TeamIntelligenceUser":false,"FOB":"","HourlyRate":-1,"LandingPage":"MapView.aspx","PreferredLanguage":"","LocationIds":[],"DepartmentIds":[],"IID":"5AB99F30-4CC9-4C74-98C0-57A426A72114"},"Subscribe":{"$type":"FI.FIC.Contracts.DataObjects.BaseObject.SubscribeMessageByEmail, FICIntfAdv","NeedSendMessages":[],"UserEmail":"","UserTextMessage":""},"Features":[{"Key":100,"Value":["99999"]},{"Key":110,"Value":["0"]},{"Key":120,"Value":["0"]},{"Key":130,"Value":["0"]},{"Key":140,"Value":["0"]},{"Key":200,"Value":["99999"]},{"Key":210,"Value":["0"]},{"Key":220,"Value":["99999"]},{"Key":230,"Value":["99999"]},{"Key":235,"Value":["99999"]},{"Key":237,"Value":["0"]},{"Key":245,"Value":["0"]},{"Key":239,"Value":["0"]},{"Key":248,"Value":["0"]},{"Key":300,"Value":["0"]},{"Key":600,"Value":["99999"]},{"Key":601,"Value":["0"]},{"Key":602,"Value":["0"]},{"Key":800,"Value":["0"]},{"Key":900,"Value":["0"]},{"Key":1000,"Value":["99999"]},{"Key":1100,"Value":["99999"]},{"Key":1101,"Value":["0"]}],"Schedule":{"$type":"FI.FIC.EmailSchedule, FICBLC","ScheduleItems":{"$type":"FI.FIC.EmailScheduleItem[], FICBLC","$values":[]}}}</t>
-  </si>
-  <si>
-    <t>{"UserInfo":{"ID":"atpermission@iicon004.com","DisplayName":"Auto+Test+Permissions","TextAddress":"","Mobile":"","BusinessPhone":"","Active":true,"UserType":"1","IsUser":true,"AllowLoginIntoPC":true,"AllowLoginIntoInspectMobile":false,"AllowLoginIntoFleetMobile":false,"AllowMobileBarcodeScanning":false,"ContactType":"100","ManagerIID":"","Notes":"","AssignedWorkOrders":false,"EmailOptOut":false,"InspectEmailList":false,"TeamIntelligenceUser":false,"FOB":"","HourlyRate":-1,"LandingPage":"MapView.aspx","PreferredLanguage":"","LocationIds":[],"DepartmentIds":[],"IID":"5AB99F30-4CC9-4C74-98C0-57A426A72114"},"Subscribe":{"$type":"FI.FIC.Contracts.DataObjects.BaseObject.SubscribeMessageByEmail, FICIntfAdv","NeedSendMessages":[],"UserEmail":"","UserTextMessage":""},"Features":[{"Key":100,"Value":["99999"]},{"Key":110,"Value":["0"]},{"Key":120,"Value":["0"]},{"Key":130,"Value":["0"]},{"Key":140,"Value":["0"]},{"Key":200,"Value":["99999"]},{"Key":210,"Value":["99999"]},{"Key":220,"Value":["99999"]},{"Key":230,"Value":["99999"]},{"Key":235,"Value":["99999"]},{"Key":237,"Value":["99999"]},{"Key":245,"Value":["99999"]},{"Key":239,"Value":["99999"]},{"Key":248,"Value":["99999"]},{"Key":300,"Value":["0"]},{"Key":600,"Value":["99999"]},{"Key":601,"Value":["0"]},{"Key":602,"Value":["0"]},{"Key":800,"Value":["0"]},{"Key":900,"Value":["0"]},{"Key":1000,"Value":["99999"]},{"Key":1100,"Value":["99999"]},{"Key":1101,"Value":["0"]}],"Schedule":{"$type":"FI.FIC.EmailSchedule, FICBLC","ScheduleItems":{"$type":"FI.FIC.EmailScheduleItem[], FICBLC","$values":[]}}}</t>
-  </si>
-  <si>
-    <t>Work Order,Alerts Management,Maintenance Schedules,Maintenance Record,Fuel Records,Customer Record,Customer Satisfaction Surveys,Survey Management/Result,Templates</t>
-  </si>
-  <si>
-    <t>{"UserInfo":{"ID":"atpermission@iicon004.com","DisplayName":"Auto+Test+Permissions","TextAddress":"","Mobile":"","BusinessPhone":"","Active":true,"UserType":"1","IsUser":true,"AllowLoginIntoPC":true,"AllowLoginIntoInspectMobile":false,"AllowLoginIntoFleetMobile":false,"AllowMobileBarcodeScanning":false,"ContactType":"100","ManagerIID":"","Notes":"","AssignedWorkOrders":false,"EmailOptOut":false,"InspectEmailList":false,"TeamIntelligenceUser":false,"FOB":"","HourlyRate":-1,"LandingPage":"MapView.aspx","PreferredLanguage":"","IsAdvisor":false,"LocationIds":[],"DepartmentIds":[],"IID":"5AB99F30-4CC9-4C74-98C0-57A426A72114"},"Subscribe":{"$type":"FI.FIC.Contracts.DataObjects.BaseObject.SubscribeMessageByEmail,+FICIntfAdv","NeedSendMessages":[],"UserEmail":"","UserTextMessage":""},"Features":[{"Key":100,"Value":["99999"]},{"Key":110,"Value":["0"]},{"Key":120,"Value":["0"]},{"Key":130,"Value":["0"]},{"Key":140,"Value":["0"]},{"Key":200,"Value":["99999"]},{"Key":210,"Value":["0"]},{"Key":220,"Value":["0"]},{"Key":230,"Value":["0"]},{"Key":235,"Value":["0"]},{"Key":237,"Value":["0"]},{"Key":245,"Value":["0"]},{"Key":239,"Value":["0"]},{"Key":248,"Value":["0"]},{"Key":300,"Value":["0"]},{"Key":600,"Value":["99999"]},{"Key":601,"Value":["0"]},{"Key":602,"Value":["0"]},{"Key":800,"Value":["99999"]},{"Key":900,"Value":["99999"]},{"Key":1000,"Value":["0"]},{"Key":1100,"Value":["0"]},{"Key":1101,"Value":["0"]}],"Schedule":{"$type":"FI.FIC.EmailSchedule,+FICBLC","ScheduleItems":{"$type":"FI.FIC.EmailScheduleItem[],+FICBLC","$values":[]}}}</t>
-  </si>
-  <si>
-    <t>{"UserInfo":{"ID":"atpermission@iicon004.com","DisplayName":"Auto+Test+Permissions","TextAddress":"","Mobile":"","BusinessPhone":"","Active":true,"UserType":"1","IsUser":true,"AllowLoginIntoPC":true,"AllowLoginIntoInspectMobile":false,"AllowLoginIntoFleetMobile":false,"AllowMobileBarcodeScanning":false,"ContactType":"100","ManagerIID":"","Notes":"","AssignedWorkOrders":false,"EmailOptOut":false,"InspectEmailList":false,"TeamIntelligenceUser":false,"FOB":"","HourlyRate":-1,"LandingPage":"MapView.aspx","PreferredLanguage":"","IsAdvisor":false,"LocationIds":[],"DepartmentIds":[],"IID":"5AB99F30-4CC9-4C74-98C0-57A426A72114"},"Subscribe":{"$type":"FI.FIC.Contracts.DataObjects.BaseObject.SubscribeMessageByEmail,+FICIntfAdv","NeedSendMessages":[],"UserEmail":"","UserTextMessage":""},"Features":[{"Key":100,"Value":["99999"]},{"Key":110,"Value":["0"]},{"Key":120,"Value":["0"]},{"Key":130,"Value":["0"]},{"Key":140,"Value":["0"]},{"Key":200,"Value":["0"]},{"Key":210,"Value":["99999"]},{"Key":220,"Value":["0"]},{"Key":230,"Value":["0"]},{"Key":235,"Value":["0"]},{"Key":237,"Value":["0"]},{"Key":245,"Value":["0"]},{"Key":239,"Value":["0"]},{"Key":248,"Value":["0"]},{"Key":300,"Value":["0"]},{"Key":600,"Value":["99999"]},{"Key":601,"Value":["0"]},{"Key":602,"Value":["0"]},{"Key":800,"Value":["99999"]},{"Key":900,"Value":["99999"]},{"Key":1000,"Value":["0"]},{"Key":1100,"Value":["0"]},{"Key":1101,"Value":["0"]}],"Schedule":{"$type":"FI.FIC.EmailSchedule,+FICBLC","ScheduleItems":{"$type":"FI.FIC.EmailScheduleItem[],+FICBLC","$values":[]}}}</t>
-  </si>
-  <si>
-    <t>{"UserInfo":{"ID":"atpermission@iicon004.com","DisplayName":"Auto+Test+Permissions","TextAddress":"","Mobile":"","BusinessPhone":"","Active":true,"UserType":"1","IsUser":true,"AllowLoginIntoPC":true,"AllowLoginIntoInspectMobile":false,"AllowLoginIntoFleetMobile":false,"AllowMobileBarcodeScanning":false,"ContactType":"100","ManagerIID":"","Notes":"","AssignedWorkOrders":false,"EmailOptOut":false,"InspectEmailList":false,"TeamIntelligenceUser":false,"FOB":"","HourlyRate":-1,"LandingPage":"MapView.aspx","PreferredLanguage":"","IsAdvisor":false,"LocationIds":[],"DepartmentIds":[],"IID":"5AB99F30-4CC9-4C74-98C0-57A426A72114"},"Subscribe":{"$type":"FI.FIC.Contracts.DataObjects.BaseObject.SubscribeMessageByEmail,+FICIntfAdv","NeedSendMessages":[],"UserEmail":"","UserTextMessage":""},"Features":[{"Key":100,"Value":["99999"]},{"Key":110,"Value":["0"]},{"Key":120,"Value":["0"]},{"Key":130,"Value":["0"]},{"Key":140,"Value":["0"]},{"Key":200,"Value":["0"]},{"Key":210,"Value":["0"]},{"Key":220,"Value":["99999"]},{"Key":230,"Value":["0"]},{"Key":235,"Value":["0"]},{"Key":237,"Value":["0"]},{"Key":245,"Value":["0"]},{"Key":239,"Value":["0"]},{"Key":248,"Value":["0"]},{"Key":300,"Value":["0"]},{"Key":600,"Value":["99999"]},{"Key":601,"Value":["0"]},{"Key":602,"Value":["0"]},{"Key":800,"Value":["99999"]},{"Key":900,"Value":["99999"]},{"Key":1000,"Value":["0"]},{"Key":1100,"Value":["0"]},{"Key":1101,"Value":["0"]}],"Schedule":{"$type":"FI.FIC.EmailSchedule,+FICBLC","ScheduleItems":{"$type":"FI.FIC.EmailScheduleItem[],+FICBLC","$values":[]}}}</t>
-  </si>
-  <si>
-    <t>{"UserInfo":{"ID":"atpermission@iicon004.com","DisplayName":"Auto+Test+Permissions","TextAddress":"","Mobile":"","BusinessPhone":"","Active":true,"UserType":"1","IsUser":true,"AllowLoginIntoPC":true,"AllowLoginIntoInspectMobile":false,"AllowLoginIntoFleetMobile":false,"AllowMobileBarcodeScanning":false,"ContactType":"100","ManagerIID":"","Notes":"","AssignedWorkOrders":false,"EmailOptOut":false,"InspectEmailList":false,"TeamIntelligenceUser":false,"FOB":"","HourlyRate":-1,"LandingPage":"MapView.aspx","PreferredLanguage":"","IsAdvisor":false,"LocationIds":[],"DepartmentIds":[],"IID":"5AB99F30-4CC9-4C74-98C0-57A426A72114"},"Subscribe":{"$type":"FI.FIC.Contracts.DataObjects.BaseObject.SubscribeMessageByEmail,+FICIntfAdv","NeedSendMessages":[],"UserEmail":"","UserTextMessage":""},"Features":[{"Key":100,"Value":["99999"]},{"Key":110,"Value":["0"]},{"Key":120,"Value":["0"]},{"Key":130,"Value":["0"]},{"Key":140,"Value":["0"]},{"Key":200,"Value":["0"]},{"Key":210,"Value":["0"]},{"Key":220,"Value":["0"]},{"Key":230,"Value":["99999"]},{"Key":235,"Value":["0"]},{"Key":237,"Value":["0"]},{"Key":245,"Value":["0"]},{"Key":239,"Value":["0"]},{"Key":248,"Value":["0"]},{"Key":300,"Value":["0"]},{"Key":600,"Value":["99999"]},{"Key":601,"Value":["0"]},{"Key":602,"Value":["0"]},{"Key":800,"Value":["99999"]},{"Key":900,"Value":["99999"]},{"Key":1000,"Value":["0"]},{"Key":1100,"Value":["0"]},{"Key":1101,"Value":["0"]}],"Schedule":{"$type":"FI.FIC.EmailSchedule,+FICBLC","ScheduleItems":{"$type":"FI.FIC.EmailScheduleItem[],+FICBLC","$values":[]}}}</t>
-  </si>
-  <si>
-    <t>{"UserInfo":{"ID":"atpermission@iicon004.com","DisplayName":"Auto+Test+Permissions","TextAddress":"","Mobile":"","BusinessPhone":"","Active":true,"UserType":"1","IsUser":true,"AllowLoginIntoPC":true,"AllowLoginIntoInspectMobile":false,"AllowLoginIntoFleetMobile":false,"AllowMobileBarcodeScanning":false,"ContactType":"100","ManagerIID":"","Notes":"","AssignedWorkOrders":false,"EmailOptOut":false,"InspectEmailList":false,"TeamIntelligenceUser":false,"FOB":"","HourlyRate":-1,"LandingPage":"MapView.aspx","PreferredLanguage":"","IsAdvisor":false,"LocationIds":[],"DepartmentIds":[],"IID":"5AB99F30-4CC9-4C74-98C0-57A426A72114"},"Subscribe":{"$type":"FI.FIC.Contracts.DataObjects.BaseObject.SubscribeMessageByEmail,+FICIntfAdv","NeedSendMessages":[],"UserEmail":"","UserTextMessage":""},"Features":[{"Key":100,"Value":["99999"]},{"Key":110,"Value":["0"]},{"Key":120,"Value":["0"]},{"Key":130,"Value":["0"]},{"Key":140,"Value":["0"]},{"Key":200,"Value":["99999"]},{"Key":210,"Value":["99999"]},{"Key":220,"Value":["0"]},{"Key":230,"Value":["0"]},{"Key":235,"Value":["0"]},{"Key":237,"Value":["0"]},{"Key":245,"Value":["0"]},{"Key":239,"Value":["0"]},{"Key":248,"Value":["0"]},{"Key":300,"Value":["0"]},{"Key":600,"Value":["99999"]},{"Key":601,"Value":["0"]},{"Key":602,"Value":["0"]},{"Key":800,"Value":["99999"]},{"Key":900,"Value":["99999"]},{"Key":1000,"Value":["0"]},{"Key":1100,"Value":["0"]},{"Key":1101,"Value":["0"]}],"Schedule":{"$type":"FI.FIC.EmailSchedule,+FICBLC","ScheduleItems":{"$type":"FI.FIC.EmailScheduleItem[],+FICBLC","$values":[]}}}</t>
-  </si>
-  <si>
-    <t>{"UserInfo":{"ID":"atpermission@iicon004.com","DisplayName":"Auto+Test+Permissions","TextAddress":"","Mobile":"","BusinessPhone":"","Active":true,"UserType":"1","IsUser":true,"AllowLoginIntoPC":true,"AllowLoginIntoInspectMobile":false,"AllowLoginIntoFleetMobile":false,"AllowMobileBarcodeScanning":false,"ContactType":"100","ManagerIID":"","Notes":"","AssignedWorkOrders":false,"EmailOptOut":false,"InspectEmailList":false,"TeamIntelligenceUser":false,"FOB":"","HourlyRate":-1,"LandingPage":"MapView.aspx","PreferredLanguage":"","IsAdvisor":false,"LocationIds":[],"DepartmentIds":[],"IID":"5AB99F30-4CC9-4C74-98C0-57A426A72114"},"Subscribe":{"$type":"FI.FIC.Contracts.DataObjects.BaseObject.SubscribeMessageByEmail,+FICIntfAdv","NeedSendMessages":[],"UserEmail":"","UserTextMessage":""},"Features":[{"Key":100,"Value":["99999"]},{"Key":110,"Value":["0"]},{"Key":120,"Value":["0"]},{"Key":130,"Value":["0"]},{"Key":140,"Value":["0"]},{"Key":200,"Value":["99999"]},{"Key":210,"Value":["0"]},{"Key":220,"Value":["99999"]},{"Key":230,"Value":["0"]},{"Key":235,"Value":["0"]},{"Key":237,"Value":["0"]},{"Key":245,"Value":["0"]},{"Key":239,"Value":["0"]},{"Key":248,"Value":["0"]},{"Key":300,"Value":["0"]},{"Key":600,"Value":["99999"]},{"Key":601,"Value":["0"]},{"Key":602,"Value":["0"]},{"Key":800,"Value":["99999"]},{"Key":900,"Value":["99999"]},{"Key":1000,"Value":["0"]},{"Key":1100,"Value":["0"]},{"Key":1101,"Value":["0"]}],"Schedule":{"$type":"FI.FIC.EmailSchedule,+FICBLC","ScheduleItems":{"$type":"FI.FIC.EmailScheduleItem[],+FICBLC","$values":[]}}}</t>
+    <t>Maintenance Schedules</t>
+  </si>
+  <si>
+    <t>Alerts Management,Maintenance Schedules</t>
+  </si>
+  <si>
+    <t>Maintenance Schedules,Customer Record</t>
+  </si>
+  <si>
+    <t>Alerts Management,Maintenance Schedules,Fuel Records,Customer Record</t>
+  </si>
+  <si>
+    <t>Work Order,Alerts Management,Maintenance Schedules,Fuel Records,Customer Record,Customer Satisfaction Surveys,Survey Management/Result,Templates,Report</t>
   </si>
 </sst>
 </file>
@@ -194,7 +185,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -210,7 +201,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -509,7 +500,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,54 +526,54 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -590,87 +581,87 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
         <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B14" t="s">
         <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>